<commit_message>
adding scene calculations initializer
</commit_message>
<xml_diff>
--- a/Projects/CCBZA_SAND/Data/Template_QSR.xlsx
+++ b/Projects/CCBZA_SAND/Data/Template_QSR.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPI" sheetId="1" state="visible" r:id="rId2"/>
@@ -91,7 +91,7 @@
     <t xml:space="preserve">Stills - IC</t>
   </si>
   <si>
-    <t xml:space="preserve">COMBO'S &amp; ACTIVATION</t>
+    <t xml:space="preserve">COMBOS &amp; ACTIVATION</t>
   </si>
   <si>
     <t xml:space="preserve">Menu Combos</t>
@@ -476,7 +476,7 @@
     <numFmt numFmtId="166" formatCode="0"/>
     <numFmt numFmtId="167" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -498,12 +498,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -568,7 +562,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -592,12 +586,8 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -618,11 +608,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -670,7 +656,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -691,14 +677,13 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -770,18 +755,18 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.4279069767442"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="35.9348837209302"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.353488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.7813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="17.8418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.4093023255814"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="36.9209302325581"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.8418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="38.8883720930233"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="18.3348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -859,7 +844,7 @@
       <c r="B4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -883,7 +868,7 @@
       <c r="B5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -907,7 +892,7 @@
       <c r="B6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -976,7 +961,7 @@
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -996,7 +981,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
@@ -1020,7 +1005,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
@@ -1111,51 +1096,51 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.9348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.4511627906977"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.1767441860465"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.86046511627907"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.96744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="9.72093023255814"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="59.3162790697674"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.4418604651163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.6558139534884"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="9.96744186046512"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="61.1627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="7"/>
+      <c r="J1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -1173,7 +1158,7 @@
       <c r="E2" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>40</v>
       </c>
       <c r="I2" s="0" t="s">
@@ -1205,73 +1190,72 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.353488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="67.8093023255814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.553488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.9813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.73953488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.8744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.4604651162791"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="6.27441860465116"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.4418604651163"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.2604651162791"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.72093023255814"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.2139534883721"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.2"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="50.4558139534884"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8418604651163"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="69.7767441860465"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.4744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.246511627907"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="6.4"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.0604651162791"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.6279069767442"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.96744186046512"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.4604651162791"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="51.9302325581395"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="6" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1291,13 +1275,13 @@
       <c r="E2" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="M2" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="Q2" s="8" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1308,34 +1292,34 @@
       <c r="B3" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="11" t="n">
+      <c r="E3" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="8" t="s">
         <v>65</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="M3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="Q3" s="9" t="s">
+      <c r="Q3" s="8" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1346,26 +1330,26 @@
       <c r="B4" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
       <c r="J4" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="M4" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="Q4" s="9" t="s">
+      <c r="Q4" s="8" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1379,13 +1363,13 @@
       <c r="J5" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="M5" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="Q5" s="9" t="s">
+      <c r="Q5" s="8" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1399,13 +1383,13 @@
       <c r="J6" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="L6" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="M6" s="10" t="s">
+      <c r="M6" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="Q6" s="9" t="s">
+      <c r="Q6" s="8" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1419,13 +1403,13 @@
       <c r="J7" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="L7" s="10" t="s">
+      <c r="L7" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="M7" s="10" t="s">
+      <c r="M7" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="Q7" s="9" t="s">
+      <c r="Q7" s="8" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1439,13 +1423,13 @@
       <c r="J8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="L8" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="M8" s="10" t="s">
+      <c r="M8" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="Q8" s="9" t="s">
+      <c r="Q8" s="8" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1459,13 +1443,13 @@
       <c r="J9" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="L9" s="10" t="s">
+      <c r="L9" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="M9" s="10" t="s">
+      <c r="M9" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="Q9" s="9" t="s">
+      <c r="Q9" s="8" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1479,13 +1463,13 @@
       <c r="J10" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="L10" s="10" t="s">
+      <c r="L10" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="M10" s="10" t="s">
+      <c r="M10" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="Q10" s="9" t="s">
+      <c r="Q10" s="8" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1499,13 +1483,13 @@
       <c r="J11" s="0" t="n">
         <v>10.5</v>
       </c>
-      <c r="L11" s="10" t="s">
+      <c r="L11" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="M11" s="10" t="s">
+      <c r="M11" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="Q11" s="9" t="s">
+      <c r="Q11" s="8" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1519,13 +1503,13 @@
       <c r="J12" s="0" t="n">
         <v>12.99</v>
       </c>
-      <c r="L12" s="10" t="s">
+      <c r="L12" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="M12" s="10" t="s">
+      <c r="M12" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="Q12" s="9" t="s">
+      <c r="Q12" s="8" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1539,13 +1523,13 @@
       <c r="J13" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="L13" s="10" t="s">
+      <c r="L13" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="M13" s="10" t="s">
+      <c r="M13" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="Q13" s="9" t="s">
+      <c r="Q13" s="8" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1559,7 +1543,7 @@
       <c r="D14" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="12" t="s">
         <v>80</v>
       </c>
       <c r="J14" s="0" t="n">
@@ -1568,13 +1552,13 @@
       <c r="K14" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="L14" s="10" t="s">
+      <c r="L14" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="M14" s="10" t="s">
+      <c r="M14" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="Q14" s="9" t="s">
+      <c r="Q14" s="8" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1585,20 +1569,20 @@
       <c r="B15" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="E15" s="14"/>
+      <c r="E15" s="13"/>
       <c r="J15" s="0" t="n">
         <v>17</v>
       </c>
       <c r="K15" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="L15" s="10" t="s">
+      <c r="L15" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="M15" s="10" t="s">
+      <c r="M15" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="Q15" s="9" t="s">
+      <c r="Q15" s="8" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1627,40 +1611,40 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="72.4837209302326"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="56.8558139534884"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.0139534883721"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.4418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.96744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.2604651162791"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.72093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="74.6976744186047"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.5767441860465"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.0604651162791"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.6279069767442"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.96744186046512"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1674,40 +1658,40 @@
       <c r="C2" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="10"/>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>86</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="10"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>87</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="10"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -1719,43 +1703,43 @@
       <c r="C5" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="10"/>
+      <c r="G5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>88</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="10"/>
+      <c r="G6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>89</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="10"/>
+      <c r="G7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="14" t="s">
         <v>29</v>
       </c>
       <c r="B8" s="0" t="s">
@@ -1764,7 +1748,7 @@
       <c r="C8" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1787,569 +1771,569 @@
   </sheetPr>
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="99.4325581395349"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3813953488372"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.3488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.6139534883721"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="16" width="93.6511627906977"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.446511627907"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.50697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.046511627907"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="102.386046511628"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.9953488372093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.0883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.106976744186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="15" width="96.4790697674419"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.8139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.62790697674419"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="5.29302325581395"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="6.27441860465116"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="5.90697674418605"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.96744186046512"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.2604651162791"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.72093023255814"/>
-    <col collapsed="false" hidden="false" max="17" min="16" style="0" width="8.86046511627907"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="60.9162790697674"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="6.4"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.02790697674419"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.2139534883721"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.6279069767442"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.96744186046512"/>
+    <col collapsed="false" hidden="false" max="17" min="16" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="62.6372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="6" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10" t="s">
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10" t="s">
+      <c r="O2" s="9"/>
+      <c r="P2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="10" t="s">
+      <c r="Q2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="9"/>
+      <c r="R2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10" t="s">
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="N3" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10" t="s">
+      <c r="O3" s="9"/>
+      <c r="P3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="Q3" s="10" t="s">
+      <c r="Q3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="R3" s="9"/>
+      <c r="R3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10" t="s">
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="N4" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10" t="s">
+      <c r="O4" s="9"/>
+      <c r="P4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="Q4" s="10" t="s">
+      <c r="Q4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="R4" s="9"/>
+      <c r="R4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10" t="s">
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="N5" s="10" t="s">
+      <c r="N5" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10" t="s">
+      <c r="O5" s="9"/>
+      <c r="P5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="Q5" s="10" t="s">
+      <c r="Q5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="R5" s="9"/>
+      <c r="R5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10" t="s">
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="N6" s="10" t="s">
+      <c r="N6" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10" t="s">
+      <c r="O6" s="9"/>
+      <c r="P6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="Q6" s="10" t="s">
+      <c r="Q6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="R6" s="9"/>
+      <c r="R6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10" t="s">
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="N7" s="10" t="s">
+      <c r="N7" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10" t="s">
+      <c r="O7" s="9"/>
+      <c r="P7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="Q7" s="10" t="s">
+      <c r="Q7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="R7" s="9"/>
+      <c r="R7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10" t="s">
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="N8" s="10" t="s">
+      <c r="N8" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10" t="s">
+      <c r="O8" s="9"/>
+      <c r="P8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="Q8" s="10" t="s">
+      <c r="Q8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="R8" s="9"/>
+      <c r="R8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10" t="n">
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10" t="s">
+      <c r="L9" s="9"/>
+      <c r="M9" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="N9" s="10" t="s">
+      <c r="N9" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10" t="s">
+      <c r="O9" s="9"/>
+      <c r="P9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="Q9" s="10" t="s">
+      <c r="Q9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="R9" s="9" t="s">
+      <c r="R9" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="H10" s="21" t="n">
+      <c r="H10" s="20" t="n">
         <v>330500</v>
       </c>
       <c r="K10" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="M10" s="10" t="s">
+      <c r="M10" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="N10" s="10" t="s">
+      <c r="N10" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10" t="s">
+      <c r="O10" s="9"/>
+      <c r="P10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="Q10" s="10" t="s">
+      <c r="Q10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="R10" s="9" t="s">
+      <c r="R10" s="8" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="M11" s="10" t="s">
+      <c r="M11" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="N11" s="10" t="s">
+      <c r="N11" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="P11" s="10" t="s">
+      <c r="P11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="Q11" s="10" t="s">
+      <c r="Q11" s="9" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="K12" s="10" t="n">
+      <c r="K12" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10" t="s">
+      <c r="L12" s="9"/>
+      <c r="M12" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="N12" s="10" t="s">
+      <c r="N12" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="P12" s="10" t="s">
+      <c r="P12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="Q12" s="10" t="s">
+      <c r="Q12" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="R12" s="9" t="s">
+      <c r="R12" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="H13" s="21" t="n">
+      <c r="H13" s="20" t="n">
         <v>330500</v>
       </c>
       <c r="K13" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="M13" s="10" t="s">
+      <c r="M13" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="N13" s="10" t="s">
+      <c r="N13" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10" t="s">
+      <c r="O13" s="9"/>
+      <c r="P13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="Q13" s="10" t="s">
+      <c r="Q13" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="R13" s="9" t="s">
+      <c r="R13" s="8" t="s">
         <v>119</v>
       </c>
     </row>
@@ -2378,81 +2362,81 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.9348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="72.8511627906977"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.3488372093023"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.3488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.8883720930233"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.9348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.6"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="37.9023255813953"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.8418604651163"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.1348837209302"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="27.9348837209302"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.6"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.4"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.96744186046512"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.753488372093"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="75.0697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.0883720930233"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.5813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.506976744186"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.0883720930233"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="39.0093023255814"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.5813953488372"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.7488372093023"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.0883720930233"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.52093023255814"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.2139534883721"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.1209302325581"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="S1" s="6" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2499,7 +2483,7 @@
       <c r="N2" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="9" t="s">
         <v>40</v>
       </c>
       <c r="R2" s="0" t="s">
@@ -2537,7 +2521,7 @@
       <c r="N3" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="O3" s="9" t="s">
         <v>40</v>
       </c>
       <c r="R3" s="0" t="s">
@@ -2572,38 +2556,38 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding per scene calculations and entering scene tables
</commit_message>
<xml_diff>
--- a/Projects/CCBZA_SAND/Data/Template_QSR.xlsx
+++ b/Projects/CCBZA_SAND/Data/Template_QSR.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="147">
   <si>
     <t xml:space="preserve">Set Name</t>
   </si>
@@ -76,43 +76,46 @@
     <t xml:space="preserve">Y</t>
   </si>
   <si>
+    <t xml:space="preserve">KEY PACK: Availability, Activation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD IC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD IC Diets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stills - IC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMBOS &amp; ACTIVATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Menu Combos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outside</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler Corner Decal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tillpoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BONUS POINTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Availability and Pricing</t>
+  </si>
+  <si>
     <t xml:space="preserve">KEY PACK: Availability, Pricing, Activation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SSD IC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Availability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SSD IC Diets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stills - IC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMBOS &amp; ACTIVATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Menu Combos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Outside</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cooler Corner Decal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tillpoint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Table</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BONUS POINTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Availability and Pricing</t>
   </si>
   <si>
     <t xml:space="preserve">Cooler</t>
@@ -756,17 +759,17 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.4093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="36.9209302325581"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.8418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="38.8883720930233"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="18.3348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.5162790697674"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="37.9023255813953"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.3348837209302"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.9953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="18.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1041,7 +1044,7 @@
         <v>11</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="F12" s="4" t="n">
         <v>15</v>
@@ -1058,7 +1061,7 @@
         <v>27</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>10</v>
@@ -1102,14 +1105,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.4418604651163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.6558139534884"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="9.10697674418605"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="9.96744186046512"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="61.1627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.5488372093023"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.2558139534884"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.4604651162791"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="10.2139534883721"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="62.8837209302326"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1117,28 +1120,28 @@
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J1" s="6"/>
     </row>
@@ -1147,10 +1150,10 @@
         <v>13</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>100</v>
@@ -1159,10 +1162,10 @@
         <v>6</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1190,20 +1193,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8418604651163"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="69.7767441860465"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.4744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.246511627907"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.706976744186"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="6.4"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.0604651162791"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.6279069767442"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.96744186046512"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.4604651162791"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.5674418604651"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="51.9302325581395"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3348837209302"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="71.8697674418605"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.046511627907"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.9674418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.7348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="6.52093023255814"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.553488372093"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.2139534883721"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.9348837209302"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="53.4093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1211,78 +1215,78 @@
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1290,37 +1294,37 @@
         <v>17</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E3" s="10" t="n">
         <v>200</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>5</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1328,13 +1332,13 @@
         <v>17</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
@@ -1344,13 +1348,13 @@
         <v>5</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1358,19 +1362,19 @@
         <v>17</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>7</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1378,19 +1382,19 @@
         <v>17</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J6" s="0" t="n">
         <v>10</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1398,19 +1402,19 @@
         <v>19</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J7" s="0" t="n">
         <v>5</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q7" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1418,19 +1422,19 @@
         <v>19</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J8" s="0" t="n">
         <v>7</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q8" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1438,113 +1442,113 @@
         <v>19</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J9" s="0" t="n">
         <v>9</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q9" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>13</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q10" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>10.5</v>
       </c>
       <c r="L11" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M11" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q11" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>12.99</v>
       </c>
       <c r="L12" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M12" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q12" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J13" s="0" t="n">
         <v>10</v>
       </c>
       <c r="L13" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M13" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q13" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J14" s="0" t="n">
         <v>14</v>
@@ -1553,21 +1557,21 @@
         <v>3</v>
       </c>
       <c r="L14" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q14" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E15" s="13"/>
       <c r="J15" s="0" t="n">
@@ -1577,13 +1581,13 @@
         <v>3</v>
       </c>
       <c r="L15" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M15" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q15" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1611,15 +1615,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="74.6976744186047"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.5767441860465"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.0604651162791"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.6279069767442"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.96744186046512"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="77.0372093023256"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.4232558139535"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.753488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.553488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.4604651162791"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.2139534883721"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1627,25 +1631,25 @@
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1653,13 +1657,13 @@
         <v>9</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G2" s="9"/>
     </row>
@@ -1668,13 +1672,13 @@
         <v>22</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>85</v>
-      </c>
       <c r="F3" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G3" s="9"/>
     </row>
@@ -1683,13 +1687,13 @@
         <v>23</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G4" s="9"/>
     </row>
@@ -1701,10 +1705,10 @@
         <v>24</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G5" s="9"/>
     </row>
@@ -1713,13 +1717,13 @@
         <v>25</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G6" s="9"/>
     </row>
@@ -1728,28 +1732,28 @@
         <v>26</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1777,23 +1781,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.046511627907"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="102.386046511628"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.9953488372093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.0883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.106976744186"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="15" width="96.4790697674419"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.8139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.62790697674419"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.293023255814"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="105.46511627907"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.7348837209302"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.8279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.6"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="15" width="99.4325581395349"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.75348837209302"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="5.29302325581395"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="6.4"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.02790697674419"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.2139534883721"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.6279069767442"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.96744186046512"/>
-    <col collapsed="false" hidden="false" max="17" min="16" style="0" width="9.10697674418605"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="62.6372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="6.52093023255814"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.15348837209302"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.4604651162791"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.2139534883721"/>
+    <col collapsed="false" hidden="false" max="17" min="16" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="64.4837209302326"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1801,55 +1805,55 @@
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1857,19 +1861,19 @@
         <v>17</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
@@ -1878,10 +1882,10 @@
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
       <c r="M2" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="O2" s="9"/>
       <c r="P2" s="9" t="s">
@@ -1894,22 +1898,22 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
@@ -1918,10 +1922,10 @@
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
       <c r="M3" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="O3" s="9"/>
       <c r="P3" s="9" t="s">
@@ -1934,22 +1938,22 @@
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -1958,10 +1962,10 @@
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
       <c r="M4" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="O4" s="9"/>
       <c r="P4" s="9" t="s">
@@ -1974,22 +1978,22 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
@@ -1998,10 +2002,10 @@
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
       <c r="M5" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="O5" s="9"/>
       <c r="P5" s="9" t="s">
@@ -2014,22 +2018,22 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
@@ -2038,10 +2042,10 @@
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
       <c r="M6" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="O6" s="9"/>
       <c r="P6" s="9" t="s">
@@ -2054,22 +2058,22 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
@@ -2078,10 +2082,10 @@
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
       <c r="M7" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="O7" s="9"/>
       <c r="P7" s="9" t="s">
@@ -2097,19 +2101,19 @@
         <v>17</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -2118,10 +2122,10 @@
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
       <c r="M8" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N8" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O8" s="9"/>
       <c r="P8" s="9" t="s">
@@ -2134,22 +2138,22 @@
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
@@ -2160,10 +2164,10 @@
       </c>
       <c r="L9" s="9"/>
       <c r="M9" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O9" s="9"/>
       <c r="P9" s="9" t="s">
@@ -2173,30 +2177,30 @@
         <v>15</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H10" s="20" t="n">
         <v>330500</v>
@@ -2205,10 +2209,10 @@
         <v>3</v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O10" s="9"/>
       <c r="P10" s="9" t="s">
@@ -2218,7 +2222,7 @@
         <v>15</v>
       </c>
       <c r="R10" s="8" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2226,25 +2230,25 @@
         <v>17</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="M11" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="P11" s="9" t="s">
         <v>11</v>
@@ -2255,32 +2259,32 @@
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="K12" s="9" t="n">
         <v>4</v>
       </c>
       <c r="L12" s="9"/>
       <c r="M12" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="P12" s="9" t="s">
         <v>11</v>
@@ -2289,30 +2293,30 @@
         <v>15</v>
       </c>
       <c r="R12" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H13" s="20" t="n">
         <v>330500</v>
@@ -2321,10 +2325,10 @@
         <v>3</v>
       </c>
       <c r="M13" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N13" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O13" s="9"/>
       <c r="P13" s="9" t="s">
@@ -2334,7 +2338,7 @@
         <v>15</v>
       </c>
       <c r="R13" s="8" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2362,23 +2366,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="75.0697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.0883720930233"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.5813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.506976744186"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.0883720930233"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="39.0093023255814"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.5813953488372"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.7488372093023"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.0883720930233"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.52093023255814"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.2139534883721"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.1209302325581"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="77.4046511627907"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.8279069767442"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.9348837209302"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.1209302325581"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.5813953488372"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="40.1162790697674"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.4418604651163"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="24.3674418604651"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.5813953488372"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.64651162790698"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.4604651162791"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.6139534883721"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2386,58 +2390,58 @@
         <v>1</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P1" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Q1" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2445,37 +2449,37 @@
         <v>13</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>85</v>
       </c>
       <c r="I2" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="K2" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="J2" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>138</v>
-      </c>
       <c r="L2" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="M2" s="0" t="n">
         <v>15</v>
@@ -2484,7 +2488,7 @@
         <v>10</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="R2" s="0" t="s">
         <v>11</v>
@@ -2498,22 +2502,22 @@
         <v>13</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>30</v>
@@ -2522,7 +2526,7 @@
         <v>15</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="R3" s="0" t="s">
         <v>11</v>
@@ -2556,7 +2560,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2564,31 +2568,31 @@
         <v>1</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing QSR template and bug in score calculation in case of dependency
</commit_message>
<xml_diff>
--- a/Projects/CCBZA_SAND/Data/Template_QSR.xlsx
+++ b/Projects/CCBZA_SAND/Data/Template_QSR.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="KPI" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,6 +19,7 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">Availability!$A$1:$S$13</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">Availability!$A$1:$S$13</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">Availability!$A$1:$S$13</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="127">
   <si>
     <t xml:space="preserve">Set Name</t>
   </si>
@@ -386,13 +387,16 @@
     <t xml:space="preserve">IMMEDIATE CONSUMPTION</t>
   </si>
   <si>
+    <t xml:space="preserve">att1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUTURE CONSUMPTION</t>
+  </si>
+  <si>
     <t xml:space="preserve">Attribute 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All Products</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FUTURE CONSUMPTION</t>
   </si>
   <si>
     <t xml:space="preserve">CCBSA SSDs - cold of which Diets/Zeros/Lights&gt;=65%</t>
@@ -717,19 +721,19 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.1023255813953"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3023255813953"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.9023255813953"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.3348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="39.9953488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.5674418604651"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="18.8279069767442"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.0883720930233"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.0418604651163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.0093023255814"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="41.2279069767442"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.1813953488372"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="19.4418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1099,19 +1103,19 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.6697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.9488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="9.35348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.4604651162791"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="10.2139534883721"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="62.8837209302326"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.1488372093023"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.7906976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="10.4604651162791"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="64.7302325581395"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1191,21 +1195,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3348837209302"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="71.8697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.046511627907"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.9674418604651"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.86046511627907"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.7348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.0744186046512"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="6.52093023255814"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.553488372093"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.2139534883721"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.706976744186"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.9348837209302"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="53.4093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8279069767442"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="74.0837209302326"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.293023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.4604651162791"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.2279069767442"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.446511627907"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="6.64651162790698"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.0418604651163"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.4883720930233"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.4604651162791"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="55.0093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1370,15 +1374,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1674418604651"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="109.525581395349"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.4232558139535"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="15.753488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.553488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.4604651162791"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.2139534883721"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.6604651162791"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="112.846511627907"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.1441860465116"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="16.1209302325581"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.0418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.4883720930233"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.4604651162791"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1719,31 +1723,31 @@
   </sheetPr>
   <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.306976744186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.1209302325581"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.8279069767442"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.0883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.106976744186"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="16" width="27.4418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="5.66046511627907"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.62790697674419"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.27441860465116"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="6.4"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.02790697674419"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.2139534883721"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.906976744186"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.96744186046512"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.35348837209302"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.24651162790698"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="34.0883720930233"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.553488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.2651162790698"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6883720930233"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.8279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.6"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="16" width="34"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="5.78604651162791"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.75348837209302"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.4"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="6.52093023255814"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.15348837209302"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.4604651162791"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.2744186046512"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.2139534883721"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.49302325581395"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="35.0744186046512"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="0" width="4.06046511627907"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2355,29 +2359,29 @@
   </sheetPr>
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.8558139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.8279069767442"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.9348837209302"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.1209302325581"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.5813953488372"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="40.1162790697674"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.4418604651163"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="24.3674418604651"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.5813953488372"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.64651162790698"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.4604651162791"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.6139534883721"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.3302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6883720930233"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.1627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.8604651162791"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.2"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="41.3488372093023"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="28.3023255813953"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.106976744186"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.2"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.76744186046512"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.106976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2468,7 +2472,7 @@
         <v>120</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="K2" s="0" t="s">
         <v>119</v>
@@ -2497,22 +2501,22 @@
         <v>14</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>77</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>65</v>
@@ -2555,9 +2559,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.35348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.506976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>